<commit_message>
Actualizacion de cronograma (completando el porcentaje)
</commit_message>
<xml_diff>
--- a/Línea Base/DPVEI/LB1/DPVEI-CP .xlsx
+++ b/Línea Base/DPVEI/LB1/DPVEI-CP .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unmsmmail-my.sharepoint.com/personal/esteban_quinonez_unmsm_edu_pe/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unmsmmail-my.sharepoint.com/personal/esteban_quinonez_unmsm_edu_pe/Documents/Escritorio/Tecnofusion/TECNOFUSION/Línea Base/DPVEI/LB1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF6AAFA8-7325-4CE1-8989-9C2F03A18181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{EF6AAFA8-7325-4CE1-8989-9C2F03A18181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4D66E04-974C-43A7-8B32-AFD1D8588998}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1517,31 +1517,31 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -1769,41 +1769,41 @@
   </sheetPr>
   <dimension ref="A1:K1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="54.140625" customWidth="1"/>
-    <col min="3" max="3" width="74.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="52.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="54.109375" customWidth="1"/>
+    <col min="3" max="3" width="74.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="5" max="5" width="52.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="41.25" customHeight="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="108"/>
+      <c r="C2" s="109"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -1915,7 +1915,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="110" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="61" t="s">
@@ -1943,7 +1943,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A11" s="109"/>
+      <c r="A11" s="101"/>
       <c r="B11" s="61" t="s">
         <v>21</v>
       </c>
@@ -1965,13 +1965,13 @@
       <c r="H11" s="97">
         <v>1</v>
       </c>
-      <c r="I11" s="102" t="s">
+      <c r="I11" s="104" t="s">
         <v>23</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="109"/>
+      <c r="A12" s="101"/>
       <c r="B12" s="62"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -1979,12 +1979,12 @@
       <c r="F12" s="71"/>
       <c r="G12" s="71"/>
       <c r="H12" s="97"/>
-      <c r="I12" s="110"/>
+      <c r="I12" s="105"/>
       <c r="J12" s="9"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A13" s="109"/>
+      <c r="A13" s="101"/>
       <c r="B13" s="61" t="s">
         <v>24</v>
       </c>
@@ -2006,14 +2006,14 @@
       <c r="H13" s="98">
         <v>1</v>
       </c>
-      <c r="I13" s="102" t="s">
+      <c r="I13" s="104" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="109"/>
+      <c r="A14" s="101"/>
       <c r="B14" s="61" t="s">
         <v>29</v>
       </c>
@@ -2033,11 +2033,11 @@
         <v>45180</v>
       </c>
       <c r="H14" s="99"/>
-      <c r="I14" s="110"/>
+      <c r="I14" s="105"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A15" s="109"/>
+      <c r="A15" s="101"/>
       <c r="B15" s="63" t="s">
         <v>33</v>
       </c>
@@ -2059,11 +2059,11 @@
       <c r="H15" s="97">
         <v>1</v>
       </c>
-      <c r="I15" s="110"/>
+      <c r="I15" s="105"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A16" s="109"/>
+      <c r="A16" s="101"/>
       <c r="B16" s="64" t="s">
         <v>36</v>
       </c>
@@ -2085,12 +2085,12 @@
       <c r="H16" s="97">
         <v>1</v>
       </c>
-      <c r="I16" s="110"/>
+      <c r="I16" s="105"/>
       <c r="J16" s="9"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="109"/>
+      <c r="A17" s="101"/>
       <c r="B17" s="64" t="s">
         <v>38</v>
       </c>
@@ -2112,12 +2112,12 @@
       <c r="H17" s="72">
         <v>1</v>
       </c>
-      <c r="I17" s="110"/>
+      <c r="I17" s="105"/>
       <c r="J17" s="9"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A18" s="109"/>
+      <c r="A18" s="101"/>
       <c r="B18" s="64" t="s">
         <v>41</v>
       </c>
@@ -2144,7 +2144,7 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A19" s="109"/>
+      <c r="A19" s="101"/>
       <c r="B19" s="64" t="s">
         <v>45</v>
       </c>
@@ -2171,7 +2171,7 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A20" s="109"/>
+      <c r="A20" s="101"/>
       <c r="B20" s="64" t="s">
         <v>49</v>
       </c>
@@ -2198,7 +2198,7 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="109"/>
+      <c r="A21" s="101"/>
       <c r="B21" s="64" t="s">
         <v>53</v>
       </c>
@@ -2225,7 +2225,7 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" s="109"/>
+      <c r="A22" s="101"/>
       <c r="B22" s="64" t="s">
         <v>56</v>
       </c>
@@ -2252,7 +2252,7 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" s="109"/>
+      <c r="A23" s="101"/>
       <c r="B23" s="64" t="s">
         <v>59</v>
       </c>
@@ -2279,7 +2279,7 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="109"/>
+      <c r="A24" s="101"/>
       <c r="B24" s="96" t="s">
         <v>62</v>
       </c>
@@ -2306,7 +2306,7 @@
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A25" s="111"/>
+      <c r="A25" s="102"/>
       <c r="B25" s="64" t="s">
         <v>66</v>
       </c>
@@ -2333,7 +2333,7 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="103" t="s">
+      <c r="A26" s="100" t="s">
         <v>70</v>
       </c>
       <c r="B26" s="64" t="s">
@@ -2362,7 +2362,7 @@
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="109"/>
+      <c r="A27" s="101"/>
       <c r="B27" s="64" t="s">
         <v>75</v>
       </c>
@@ -2384,14 +2384,14 @@
       <c r="H27" s="72">
         <v>1</v>
       </c>
-      <c r="I27" s="102" t="s">
+      <c r="I27" s="104" t="s">
         <v>78</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="109"/>
+      <c r="A28" s="101"/>
       <c r="B28" s="64" t="s">
         <v>79</v>
       </c>
@@ -2410,13 +2410,15 @@
       <c r="G28" s="71">
         <v>45190</v>
       </c>
-      <c r="H28" s="72"/>
-      <c r="I28" s="110"/>
+      <c r="H28" s="72">
+        <v>1</v>
+      </c>
+      <c r="I28" s="105"/>
       <c r="J28" s="9"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="109"/>
+      <c r="A29" s="101"/>
       <c r="B29" s="65" t="s">
         <v>82</v>
       </c>
@@ -2438,12 +2440,12 @@
       <c r="H29" s="72">
         <v>1</v>
       </c>
-      <c r="I29" s="110"/>
+      <c r="I29" s="105"/>
       <c r="J29" s="9"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="109"/>
+      <c r="A30" s="101"/>
       <c r="B30" s="65" t="s">
         <v>85</v>
       </c>
@@ -2462,7 +2464,7 @@
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="109"/>
+      <c r="A31" s="101"/>
       <c r="B31" s="64" t="s">
         <v>87</v>
       </c>
@@ -2481,15 +2483,17 @@
       <c r="G31" s="71">
         <v>45193</v>
       </c>
-      <c r="H31" s="72"/>
-      <c r="I31" s="102" t="s">
+      <c r="H31" s="72">
+        <v>1</v>
+      </c>
+      <c r="I31" s="104" t="s">
         <v>90</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A32" s="111"/>
+      <c r="A32" s="102"/>
       <c r="B32" s="64" t="s">
         <v>91</v>
       </c>
@@ -2508,8 +2512,10 @@
       <c r="G32" s="71">
         <v>45193</v>
       </c>
-      <c r="H32" s="72"/>
-      <c r="I32" s="110"/>
+      <c r="H32" s="72">
+        <v>1</v>
+      </c>
+      <c r="I32" s="105"/>
       <c r="J32" s="9"/>
       <c r="K32" s="2"/>
     </row>
@@ -2527,11 +2533,13 @@
       <c r="G33" s="75">
         <v>45193</v>
       </c>
-      <c r="H33" s="76"/>
-      <c r="I33" s="110"/>
+      <c r="H33" s="76">
+        <v>1</v>
+      </c>
+      <c r="I33" s="105"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="104" t="s">
+      <c r="A34" s="103" t="s">
         <v>96</v>
       </c>
       <c r="B34" s="67" t="s">
@@ -2553,14 +2561,14 @@
         <v>45199</v>
       </c>
       <c r="H34" s="77"/>
-      <c r="I34" s="102" t="s">
+      <c r="I34" s="104" t="s">
         <v>100</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="109"/>
+      <c r="A35" s="101"/>
       <c r="B35" s="67" t="s">
         <v>101</v>
       </c>
@@ -2580,12 +2588,12 @@
         <v>45199</v>
       </c>
       <c r="H35" s="77"/>
-      <c r="I35" s="110"/>
+      <c r="I35" s="105"/>
       <c r="J35" s="9"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="109"/>
+      <c r="A36" s="101"/>
       <c r="B36" s="67" t="s">
         <v>105</v>
       </c>
@@ -2605,12 +2613,12 @@
         <v>45199</v>
       </c>
       <c r="H36" s="77"/>
-      <c r="I36" s="110"/>
+      <c r="I36" s="105"/>
       <c r="J36" s="9"/>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="109"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="64" t="s">
         <v>108</v>
       </c>
@@ -2630,12 +2638,12 @@
         <v>45208</v>
       </c>
       <c r="H37" s="77"/>
-      <c r="I37" s="110"/>
+      <c r="I37" s="105"/>
       <c r="J37" s="9"/>
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A38" s="109"/>
+      <c r="A38" s="101"/>
       <c r="B38" s="64" t="s">
         <v>112</v>
       </c>
@@ -2655,12 +2663,12 @@
         <v>45208</v>
       </c>
       <c r="H38" s="72"/>
-      <c r="I38" s="110"/>
+      <c r="I38" s="105"/>
       <c r="J38" s="9"/>
       <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="109"/>
+      <c r="A39" s="101"/>
       <c r="B39" s="64" t="s">
         <v>87</v>
       </c>
@@ -2680,14 +2688,14 @@
         <v>45205</v>
       </c>
       <c r="H39" s="72"/>
-      <c r="I39" s="102" t="s">
+      <c r="I39" s="104" t="s">
         <v>117</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="41.25" customHeight="1">
-      <c r="A40" s="111"/>
+      <c r="A40" s="102"/>
       <c r="B40" s="64" t="s">
         <v>91</v>
       </c>
@@ -2707,7 +2715,7 @@
         <v>45210</v>
       </c>
       <c r="H40" s="72"/>
-      <c r="I40" s="110"/>
+      <c r="I40" s="105"/>
       <c r="J40" s="9"/>
       <c r="K40" s="2"/>
     </row>
@@ -2728,10 +2736,10 @@
         <v>45210</v>
       </c>
       <c r="H41" s="80"/>
-      <c r="I41" s="110"/>
+      <c r="I41" s="105"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A42" s="104" t="s">
+      <c r="A42" s="103" t="s">
         <v>122</v>
       </c>
       <c r="B42" s="67" t="s">
@@ -2753,12 +2761,12 @@
         <v>45218</v>
       </c>
       <c r="H42" s="72"/>
-      <c r="I42" s="102"/>
+      <c r="I42" s="104"/>
       <c r="J42" s="9"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A43" s="109"/>
+      <c r="A43" s="101"/>
       <c r="B43" s="68" t="s">
         <v>125</v>
       </c>
@@ -2778,12 +2786,12 @@
         <v>45218</v>
       </c>
       <c r="H43" s="72"/>
-      <c r="I43" s="110"/>
+      <c r="I43" s="105"/>
       <c r="J43" s="9"/>
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A44" s="109"/>
+      <c r="A44" s="101"/>
       <c r="B44" s="69" t="s">
         <v>128</v>
       </c>
@@ -2803,12 +2811,12 @@
         <v>45218</v>
       </c>
       <c r="H44" s="72"/>
-      <c r="I44" s="110"/>
+      <c r="I44" s="105"/>
       <c r="J44" s="9"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A45" s="109"/>
+      <c r="A45" s="101"/>
       <c r="B45" s="61" t="s">
         <v>130</v>
       </c>
@@ -2828,12 +2836,12 @@
         <v>45226</v>
       </c>
       <c r="H45" s="72"/>
-      <c r="I45" s="110"/>
+      <c r="I45" s="105"/>
       <c r="J45" s="9"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A46" s="109"/>
+      <c r="A46" s="101"/>
       <c r="B46" s="61" t="s">
         <v>132</v>
       </c>
@@ -2853,14 +2861,14 @@
         <v>45236</v>
       </c>
       <c r="H46" s="72"/>
-      <c r="I46" s="102" t="s">
+      <c r="I46" s="104" t="s">
         <v>135</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A47" s="109"/>
+      <c r="A47" s="101"/>
       <c r="B47" s="61" t="s">
         <v>87</v>
       </c>
@@ -2880,12 +2888,12 @@
         <v>45236</v>
       </c>
       <c r="H47" s="72"/>
-      <c r="I47" s="110"/>
+      <c r="I47" s="105"/>
       <c r="J47" s="9"/>
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A48" s="109"/>
+      <c r="A48" s="101"/>
       <c r="B48" s="61" t="s">
         <v>91</v>
       </c>
@@ -2905,14 +2913,14 @@
         <v>45244</v>
       </c>
       <c r="H48" s="72"/>
-      <c r="I48" s="102" t="s">
+      <c r="I48" s="104" t="s">
         <v>139</v>
       </c>
       <c r="J48" s="9"/>
       <c r="K48" s="2"/>
     </row>
     <row r="49" spans="1:11" ht="43.5" customHeight="1">
-      <c r="A49" s="109"/>
+      <c r="A49" s="101"/>
       <c r="B49" s="61" t="s">
         <v>140</v>
       </c>
@@ -2932,12 +2940,12 @@
         <v>45247</v>
       </c>
       <c r="H49" s="72"/>
-      <c r="I49" s="110"/>
+      <c r="I49" s="105"/>
       <c r="J49" s="9"/>
       <c r="K49" s="2"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A50" s="111"/>
+      <c r="A50" s="102"/>
       <c r="B50" s="61" t="s">
         <v>143</v>
       </c>
@@ -2957,7 +2965,7 @@
         <v>45249</v>
       </c>
       <c r="H50" s="72"/>
-      <c r="I50" s="110"/>
+      <c r="I50" s="105"/>
       <c r="J50" s="9"/>
       <c r="K50" s="2"/>
     </row>
@@ -2978,7 +2986,7 @@
         <v>45249</v>
       </c>
       <c r="H51" s="82"/>
-      <c r="I51" s="110"/>
+      <c r="I51" s="105"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1">
       <c r="B52" s="11"/>
@@ -4742,6 +4750,11 @@
     <row r="1006" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A10:A25"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I17"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A34:A40"/>
     <mergeCell ref="A42:A50"/>
@@ -4752,11 +4765,6 @@
     <mergeCell ref="I48:I51"/>
     <mergeCell ref="I27:I29"/>
     <mergeCell ref="I31:I33"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A10:A25"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -4774,12 +4782,12 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" customWidth="1"/>
-    <col min="4" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" customHeight="1"/>
@@ -4788,7 +4796,7 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="111" t="s">
         <v>148</v>
       </c>
       <c r="C3" s="112"/>

</xml_diff>

<commit_message>
estructura base de la pagina y tambien el header
</commit_message>
<xml_diff>
--- a/Línea Base/DPVEI/LB1/DPVEI-CP .xlsx
+++ b/Línea Base/DPVEI/LB1/DPVEI-CP .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unmsmmail-my.sharepoint.com/personal/esteban_quinonez_unmsm_edu_pe/Documents/Escritorio/Tecnofusion/TECNOFUSION/Línea Base/DPVEI/LB1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{EF6AAFA8-7325-4CE1-8989-9C2F03A18181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4D66E04-974C-43A7-8B32-AFD1D8588998}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{EF6AAFA8-7325-4CE1-8989-9C2F03A18181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DB3B166-70C1-478D-847F-BB4C62DC1D72}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="38">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -774,6 +774,13 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1312,7 +1319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1517,18 +1524,6 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1538,10 +1533,23 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -1563,6 +1571,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1769,8 +1781,8 @@
   </sheetPr>
   <dimension ref="A1:K1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1787,23 +1799,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="41.25" customHeight="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="109"/>
+      <c r="C2" s="103"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -1915,7 +1927,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="110" t="s">
+      <c r="A10" s="104" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="61" t="s">
@@ -1943,7 +1955,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A11" s="101"/>
+      <c r="A11" s="105"/>
       <c r="B11" s="61" t="s">
         <v>21</v>
       </c>
@@ -1965,13 +1977,13 @@
       <c r="H11" s="97">
         <v>1</v>
       </c>
-      <c r="I11" s="104" t="s">
+      <c r="I11" s="107" t="s">
         <v>23</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="101"/>
+      <c r="A12" s="105"/>
       <c r="B12" s="62"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -1979,12 +1991,12 @@
       <c r="F12" s="71"/>
       <c r="G12" s="71"/>
       <c r="H12" s="97"/>
-      <c r="I12" s="105"/>
+      <c r="I12" s="108"/>
       <c r="J12" s="9"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A13" s="101"/>
+      <c r="A13" s="105"/>
       <c r="B13" s="61" t="s">
         <v>24</v>
       </c>
@@ -2006,14 +2018,14 @@
       <c r="H13" s="98">
         <v>1</v>
       </c>
-      <c r="I13" s="104" t="s">
+      <c r="I13" s="107" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="101"/>
+      <c r="A14" s="105"/>
       <c r="B14" s="61" t="s">
         <v>29</v>
       </c>
@@ -2033,11 +2045,11 @@
         <v>45180</v>
       </c>
       <c r="H14" s="99"/>
-      <c r="I14" s="105"/>
+      <c r="I14" s="108"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A15" s="101"/>
+      <c r="A15" s="105"/>
       <c r="B15" s="63" t="s">
         <v>33</v>
       </c>
@@ -2059,11 +2071,11 @@
       <c r="H15" s="97">
         <v>1</v>
       </c>
-      <c r="I15" s="105"/>
+      <c r="I15" s="108"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A16" s="101"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="64" t="s">
         <v>36</v>
       </c>
@@ -2085,12 +2097,12 @@
       <c r="H16" s="97">
         <v>1</v>
       </c>
-      <c r="I16" s="105"/>
+      <c r="I16" s="108"/>
       <c r="J16" s="9"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="101"/>
+      <c r="A17" s="105"/>
       <c r="B17" s="64" t="s">
         <v>38</v>
       </c>
@@ -2112,12 +2124,12 @@
       <c r="H17" s="72">
         <v>1</v>
       </c>
-      <c r="I17" s="105"/>
+      <c r="I17" s="108"/>
       <c r="J17" s="9"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A18" s="101"/>
+      <c r="A18" s="105"/>
       <c r="B18" s="64" t="s">
         <v>41</v>
       </c>
@@ -2144,7 +2156,7 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A19" s="101"/>
+      <c r="A19" s="105"/>
       <c r="B19" s="64" t="s">
         <v>45</v>
       </c>
@@ -2171,7 +2183,7 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A20" s="101"/>
+      <c r="A20" s="105"/>
       <c r="B20" s="64" t="s">
         <v>49</v>
       </c>
@@ -2198,7 +2210,7 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="101"/>
+      <c r="A21" s="105"/>
       <c r="B21" s="64" t="s">
         <v>53</v>
       </c>
@@ -2225,7 +2237,7 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" s="101"/>
+      <c r="A22" s="105"/>
       <c r="B22" s="64" t="s">
         <v>56</v>
       </c>
@@ -2252,7 +2264,7 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" s="101"/>
+      <c r="A23" s="105"/>
       <c r="B23" s="64" t="s">
         <v>59</v>
       </c>
@@ -2279,7 +2291,7 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="101"/>
+      <c r="A24" s="105"/>
       <c r="B24" s="96" t="s">
         <v>62</v>
       </c>
@@ -2306,7 +2318,7 @@
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A25" s="102"/>
+      <c r="A25" s="106"/>
       <c r="B25" s="64" t="s">
         <v>66</v>
       </c>
@@ -2333,7 +2345,7 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="100" t="s">
+      <c r="A26" s="109" t="s">
         <v>70</v>
       </c>
       <c r="B26" s="64" t="s">
@@ -2362,7 +2374,7 @@
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="101"/>
+      <c r="A27" s="105"/>
       <c r="B27" s="64" t="s">
         <v>75</v>
       </c>
@@ -2384,14 +2396,14 @@
       <c r="H27" s="72">
         <v>1</v>
       </c>
-      <c r="I27" s="104" t="s">
+      <c r="I27" s="107" t="s">
         <v>78</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="101"/>
+      <c r="A28" s="105"/>
       <c r="B28" s="64" t="s">
         <v>79</v>
       </c>
@@ -2413,12 +2425,12 @@
       <c r="H28" s="72">
         <v>1</v>
       </c>
-      <c r="I28" s="105"/>
+      <c r="I28" s="108"/>
       <c r="J28" s="9"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="101"/>
+      <c r="A29" s="105"/>
       <c r="B29" s="65" t="s">
         <v>82</v>
       </c>
@@ -2440,12 +2452,12 @@
       <c r="H29" s="72">
         <v>1</v>
       </c>
-      <c r="I29" s="105"/>
+      <c r="I29" s="108"/>
       <c r="J29" s="9"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="101"/>
+      <c r="A30" s="105"/>
       <c r="B30" s="65" t="s">
         <v>85</v>
       </c>
@@ -2464,7 +2476,7 @@
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="101"/>
+      <c r="A31" s="105"/>
       <c r="B31" s="64" t="s">
         <v>87</v>
       </c>
@@ -2486,14 +2498,14 @@
       <c r="H31" s="72">
         <v>1</v>
       </c>
-      <c r="I31" s="104" t="s">
+      <c r="I31" s="107" t="s">
         <v>90</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A32" s="102"/>
+      <c r="A32" s="106"/>
       <c r="B32" s="64" t="s">
         <v>91</v>
       </c>
@@ -2515,7 +2527,7 @@
       <c r="H32" s="72">
         <v>1</v>
       </c>
-      <c r="I32" s="105"/>
+      <c r="I32" s="108"/>
       <c r="J32" s="9"/>
       <c r="K32" s="2"/>
     </row>
@@ -2536,10 +2548,10 @@
       <c r="H33" s="76">
         <v>1</v>
       </c>
-      <c r="I33" s="105"/>
+      <c r="I33" s="108"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="103" t="s">
+      <c r="A34" s="110" t="s">
         <v>96</v>
       </c>
       <c r="B34" s="67" t="s">
@@ -2561,14 +2573,14 @@
         <v>45199</v>
       </c>
       <c r="H34" s="77"/>
-      <c r="I34" s="104" t="s">
+      <c r="I34" s="107" t="s">
         <v>100</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="101"/>
+      <c r="A35" s="105"/>
       <c r="B35" s="67" t="s">
         <v>101</v>
       </c>
@@ -2588,12 +2600,12 @@
         <v>45199</v>
       </c>
       <c r="H35" s="77"/>
-      <c r="I35" s="105"/>
+      <c r="I35" s="108"/>
       <c r="J35" s="9"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="101"/>
+      <c r="A36" s="105"/>
       <c r="B36" s="67" t="s">
         <v>105</v>
       </c>
@@ -2612,13 +2624,15 @@
       <c r="G36" s="71">
         <v>45199</v>
       </c>
-      <c r="H36" s="77"/>
-      <c r="I36" s="105"/>
+      <c r="H36" s="77">
+        <v>1</v>
+      </c>
+      <c r="I36" s="108"/>
       <c r="J36" s="9"/>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="101"/>
+      <c r="A37" s="105"/>
       <c r="B37" s="64" t="s">
         <v>108</v>
       </c>
@@ -2637,13 +2651,15 @@
       <c r="G37" s="71">
         <v>45208</v>
       </c>
-      <c r="H37" s="77"/>
-      <c r="I37" s="105"/>
+      <c r="H37" s="77">
+        <v>1</v>
+      </c>
+      <c r="I37" s="108"/>
       <c r="J37" s="9"/>
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A38" s="101"/>
+      <c r="A38" s="105"/>
       <c r="B38" s="64" t="s">
         <v>112</v>
       </c>
@@ -2663,12 +2679,12 @@
         <v>45208</v>
       </c>
       <c r="H38" s="72"/>
-      <c r="I38" s="105"/>
+      <c r="I38" s="108"/>
       <c r="J38" s="9"/>
-      <c r="K38" s="2"/>
+      <c r="K38" s="113"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="101"/>
+      <c r="A39" s="105"/>
       <c r="B39" s="64" t="s">
         <v>87</v>
       </c>
@@ -2688,14 +2704,14 @@
         <v>45205</v>
       </c>
       <c r="H39" s="72"/>
-      <c r="I39" s="104" t="s">
+      <c r="I39" s="107" t="s">
         <v>117</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="41.25" customHeight="1">
-      <c r="A40" s="102"/>
+      <c r="A40" s="106"/>
       <c r="B40" s="64" t="s">
         <v>91</v>
       </c>
@@ -2715,7 +2731,7 @@
         <v>45210</v>
       </c>
       <c r="H40" s="72"/>
-      <c r="I40" s="105"/>
+      <c r="I40" s="108"/>
       <c r="J40" s="9"/>
       <c r="K40" s="2"/>
     </row>
@@ -2736,10 +2752,10 @@
         <v>45210</v>
       </c>
       <c r="H41" s="80"/>
-      <c r="I41" s="105"/>
+      <c r="I41" s="108"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A42" s="103" t="s">
+      <c r="A42" s="110" t="s">
         <v>122</v>
       </c>
       <c r="B42" s="67" t="s">
@@ -2761,12 +2777,12 @@
         <v>45218</v>
       </c>
       <c r="H42" s="72"/>
-      <c r="I42" s="104"/>
+      <c r="I42" s="107"/>
       <c r="J42" s="9"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A43" s="101"/>
+      <c r="A43" s="105"/>
       <c r="B43" s="68" t="s">
         <v>125</v>
       </c>
@@ -2786,12 +2802,12 @@
         <v>45218</v>
       </c>
       <c r="H43" s="72"/>
-      <c r="I43" s="105"/>
+      <c r="I43" s="108"/>
       <c r="J43" s="9"/>
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A44" s="101"/>
+      <c r="A44" s="105"/>
       <c r="B44" s="69" t="s">
         <v>128</v>
       </c>
@@ -2811,12 +2827,12 @@
         <v>45218</v>
       </c>
       <c r="H44" s="72"/>
-      <c r="I44" s="105"/>
+      <c r="I44" s="108"/>
       <c r="J44" s="9"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A45" s="101"/>
+      <c r="A45" s="105"/>
       <c r="B45" s="61" t="s">
         <v>130</v>
       </c>
@@ -2836,12 +2852,12 @@
         <v>45226</v>
       </c>
       <c r="H45" s="72"/>
-      <c r="I45" s="105"/>
+      <c r="I45" s="108"/>
       <c r="J45" s="9"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A46" s="101"/>
+      <c r="A46" s="105"/>
       <c r="B46" s="61" t="s">
         <v>132</v>
       </c>
@@ -2861,14 +2877,14 @@
         <v>45236</v>
       </c>
       <c r="H46" s="72"/>
-      <c r="I46" s="104" t="s">
+      <c r="I46" s="107" t="s">
         <v>135</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A47" s="101"/>
+      <c r="A47" s="105"/>
       <c r="B47" s="61" t="s">
         <v>87</v>
       </c>
@@ -2888,12 +2904,12 @@
         <v>45236</v>
       </c>
       <c r="H47" s="72"/>
-      <c r="I47" s="105"/>
+      <c r="I47" s="108"/>
       <c r="J47" s="9"/>
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A48" s="101"/>
+      <c r="A48" s="105"/>
       <c r="B48" s="61" t="s">
         <v>91</v>
       </c>
@@ -2913,14 +2929,14 @@
         <v>45244</v>
       </c>
       <c r="H48" s="72"/>
-      <c r="I48" s="104" t="s">
+      <c r="I48" s="107" t="s">
         <v>139</v>
       </c>
       <c r="J48" s="9"/>
       <c r="K48" s="2"/>
     </row>
     <row r="49" spans="1:11" ht="43.5" customHeight="1">
-      <c r="A49" s="101"/>
+      <c r="A49" s="105"/>
       <c r="B49" s="61" t="s">
         <v>140</v>
       </c>
@@ -2940,12 +2956,12 @@
         <v>45247</v>
       </c>
       <c r="H49" s="72"/>
-      <c r="I49" s="105"/>
+      <c r="I49" s="108"/>
       <c r="J49" s="9"/>
       <c r="K49" s="2"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A50" s="102"/>
+      <c r="A50" s="106"/>
       <c r="B50" s="61" t="s">
         <v>143</v>
       </c>
@@ -2965,7 +2981,7 @@
         <v>45249</v>
       </c>
       <c r="H50" s="72"/>
-      <c r="I50" s="105"/>
+      <c r="I50" s="108"/>
       <c r="J50" s="9"/>
       <c r="K50" s="2"/>
     </row>
@@ -2986,7 +3002,7 @@
         <v>45249</v>
       </c>
       <c r="H51" s="82"/>
-      <c r="I51" s="105"/>
+      <c r="I51" s="108"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1">
       <c r="B52" s="11"/>
@@ -4750,11 +4766,6 @@
     <row r="1006" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A10:A25"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I17"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A34:A40"/>
     <mergeCell ref="A42:A50"/>
@@ -4765,6 +4776,11 @@
     <mergeCell ref="I48:I51"/>
     <mergeCell ref="I27:I29"/>
     <mergeCell ref="I31:I33"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A10:A25"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
agregacion de las peticiones de cambio
</commit_message>
<xml_diff>
--- a/Línea Base/DPVEI/LB1/DPVEI-CP .xlsx
+++ b/Línea Base/DPVEI/LB1/DPVEI-CP .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unmsmmail-my.sharepoint.com/personal/esteban_quinonez_unmsm_edu_pe/Documents/Escritorio/Tecnofusion/TECNOFUSION/Línea Base/DPVEI/LB1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{EF6AAFA8-7325-4CE1-8989-9C2F03A18181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A488CB91-77B6-43D2-8740-55EDE6FBDC40}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{EF6AAFA8-7325-4CE1-8989-9C2F03A18181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D47B640-C111-481A-AA72-BBE0E3195CDD}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1534,18 +1534,6 @@
     <xf numFmtId="0" fontId="39" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1554,6 +1542,18 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1790,8 +1790,8 @@
   </sheetPr>
   <dimension ref="A1:K1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="C26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1808,23 +1808,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="41.25" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="112"/>
+      <c r="C2" s="106"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -1936,7 +1936,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="107" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="61" t="s">
@@ -1964,7 +1964,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A11" s="104"/>
+      <c r="A11" s="108"/>
       <c r="B11" s="61" t="s">
         <v>21</v>
       </c>
@@ -1986,13 +1986,13 @@
       <c r="H11" s="97">
         <v>1</v>
       </c>
-      <c r="I11" s="107" t="s">
+      <c r="I11" s="110" t="s">
         <v>23</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="104"/>
+      <c r="A12" s="108"/>
       <c r="B12" s="62"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -2000,12 +2000,12 @@
       <c r="F12" s="71"/>
       <c r="G12" s="71"/>
       <c r="H12" s="97"/>
-      <c r="I12" s="108"/>
+      <c r="I12" s="111"/>
       <c r="J12" s="9"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A13" s="104"/>
+      <c r="A13" s="108"/>
       <c r="B13" s="61" t="s">
         <v>24</v>
       </c>
@@ -2027,14 +2027,14 @@
       <c r="H13" s="98">
         <v>1</v>
       </c>
-      <c r="I13" s="107" t="s">
+      <c r="I13" s="110" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="104"/>
+      <c r="A14" s="108"/>
       <c r="B14" s="61" t="s">
         <v>29</v>
       </c>
@@ -2054,11 +2054,11 @@
         <v>45180</v>
       </c>
       <c r="H14" s="99"/>
-      <c r="I14" s="108"/>
+      <c r="I14" s="111"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A15" s="104"/>
+      <c r="A15" s="108"/>
       <c r="B15" s="63" t="s">
         <v>33</v>
       </c>
@@ -2080,11 +2080,11 @@
       <c r="H15" s="97">
         <v>1</v>
       </c>
-      <c r="I15" s="108"/>
+      <c r="I15" s="111"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A16" s="104"/>
+      <c r="A16" s="108"/>
       <c r="B16" s="64" t="s">
         <v>36</v>
       </c>
@@ -2106,12 +2106,12 @@
       <c r="H16" s="97">
         <v>1</v>
       </c>
-      <c r="I16" s="108"/>
+      <c r="I16" s="111"/>
       <c r="J16" s="9"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="104"/>
+      <c r="A17" s="108"/>
       <c r="B17" s="64" t="s">
         <v>38</v>
       </c>
@@ -2133,12 +2133,12 @@
       <c r="H17" s="72">
         <v>1</v>
       </c>
-      <c r="I17" s="108"/>
+      <c r="I17" s="111"/>
       <c r="J17" s="9"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A18" s="104"/>
+      <c r="A18" s="108"/>
       <c r="B18" s="64" t="s">
         <v>41</v>
       </c>
@@ -2165,7 +2165,7 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A19" s="104"/>
+      <c r="A19" s="108"/>
       <c r="B19" s="64" t="s">
         <v>45</v>
       </c>
@@ -2192,7 +2192,7 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A20" s="104"/>
+      <c r="A20" s="108"/>
       <c r="B20" s="64" t="s">
         <v>49</v>
       </c>
@@ -2219,7 +2219,7 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="104"/>
+      <c r="A21" s="108"/>
       <c r="B21" s="64" t="s">
         <v>53</v>
       </c>
@@ -2246,7 +2246,7 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" s="104"/>
+      <c r="A22" s="108"/>
       <c r="B22" s="64" t="s">
         <v>56</v>
       </c>
@@ -2273,7 +2273,7 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" s="104"/>
+      <c r="A23" s="108"/>
       <c r="B23" s="64" t="s">
         <v>59</v>
       </c>
@@ -2300,7 +2300,7 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="104"/>
+      <c r="A24" s="108"/>
       <c r="B24" s="96" t="s">
         <v>62</v>
       </c>
@@ -2327,7 +2327,7 @@
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A25" s="105"/>
+      <c r="A25" s="109"/>
       <c r="B25" s="64" t="s">
         <v>66</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="103" t="s">
+      <c r="A26" s="112" t="s">
         <v>70</v>
       </c>
       <c r="B26" s="64" t="s">
@@ -2383,7 +2383,7 @@
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="104"/>
+      <c r="A27" s="108"/>
       <c r="B27" s="64" t="s">
         <v>75</v>
       </c>
@@ -2405,14 +2405,14 @@
       <c r="H27" s="72">
         <v>1</v>
       </c>
-      <c r="I27" s="107" t="s">
+      <c r="I27" s="110" t="s">
         <v>78</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="104"/>
+      <c r="A28" s="108"/>
       <c r="B28" s="64" t="s">
         <v>79</v>
       </c>
@@ -2434,12 +2434,12 @@
       <c r="H28" s="72">
         <v>1</v>
       </c>
-      <c r="I28" s="108"/>
+      <c r="I28" s="111"/>
       <c r="J28" s="9"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="104"/>
+      <c r="A29" s="108"/>
       <c r="B29" s="65" t="s">
         <v>82</v>
       </c>
@@ -2461,12 +2461,12 @@
       <c r="H29" s="72">
         <v>1</v>
       </c>
-      <c r="I29" s="108"/>
+      <c r="I29" s="111"/>
       <c r="J29" s="9"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="104"/>
+      <c r="A30" s="108"/>
       <c r="B30" s="65" t="s">
         <v>85</v>
       </c>
@@ -2485,7 +2485,7 @@
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="104"/>
+      <c r="A31" s="108"/>
       <c r="B31" s="64" t="s">
         <v>87</v>
       </c>
@@ -2507,14 +2507,14 @@
       <c r="H31" s="72">
         <v>1</v>
       </c>
-      <c r="I31" s="107" t="s">
+      <c r="I31" s="110" t="s">
         <v>90</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A32" s="105"/>
+      <c r="A32" s="109"/>
       <c r="B32" s="64" t="s">
         <v>91</v>
       </c>
@@ -2536,7 +2536,7 @@
       <c r="H32" s="72">
         <v>1</v>
       </c>
-      <c r="I32" s="108"/>
+      <c r="I32" s="111"/>
       <c r="J32" s="9"/>
       <c r="K32" s="2"/>
     </row>
@@ -2557,10 +2557,10 @@
       <c r="H33" s="76">
         <v>1</v>
       </c>
-      <c r="I33" s="108"/>
+      <c r="I33" s="111"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="106" t="s">
+      <c r="A34" s="113" t="s">
         <v>96</v>
       </c>
       <c r="B34" s="67" t="s">
@@ -2582,14 +2582,14 @@
         <v>45199</v>
       </c>
       <c r="H34" s="77"/>
-      <c r="I34" s="107" t="s">
+      <c r="I34" s="110" t="s">
         <v>100</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="104"/>
+      <c r="A35" s="108"/>
       <c r="B35" s="67" t="s">
         <v>101</v>
       </c>
@@ -2611,12 +2611,12 @@
       <c r="H35" s="77">
         <v>1</v>
       </c>
-      <c r="I35" s="108"/>
+      <c r="I35" s="111"/>
       <c r="J35" s="9"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="104"/>
+      <c r="A36" s="108"/>
       <c r="B36" s="67" t="s">
         <v>105</v>
       </c>
@@ -2638,12 +2638,12 @@
       <c r="H36" s="77">
         <v>1</v>
       </c>
-      <c r="I36" s="108"/>
+      <c r="I36" s="111"/>
       <c r="J36" s="9"/>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="104"/>
+      <c r="A37" s="108"/>
       <c r="B37" s="64" t="s">
         <v>108</v>
       </c>
@@ -2665,12 +2665,12 @@
       <c r="H37" s="77">
         <v>1</v>
       </c>
-      <c r="I37" s="108"/>
+      <c r="I37" s="111"/>
       <c r="J37" s="9"/>
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A38" s="104"/>
+      <c r="A38" s="108"/>
       <c r="B38" s="64" t="s">
         <v>112</v>
       </c>
@@ -2692,12 +2692,12 @@
       <c r="H38" s="77">
         <v>1</v>
       </c>
-      <c r="I38" s="108"/>
+      <c r="I38" s="111"/>
       <c r="J38" s="9"/>
       <c r="K38" s="100"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="104"/>
+      <c r="A39" s="108"/>
       <c r="B39" s="64" t="s">
         <v>87</v>
       </c>
@@ -2719,14 +2719,14 @@
       <c r="H39" s="77">
         <v>1</v>
       </c>
-      <c r="I39" s="107" t="s">
+      <c r="I39" s="110" t="s">
         <v>117</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="41.25" customHeight="1">
-      <c r="A40" s="105"/>
+      <c r="A40" s="109"/>
       <c r="B40" s="64" t="s">
         <v>91</v>
       </c>
@@ -2748,7 +2748,7 @@
       <c r="H40" s="72">
         <v>1</v>
       </c>
-      <c r="I40" s="108"/>
+      <c r="I40" s="111"/>
       <c r="J40" s="9"/>
       <c r="K40" s="2"/>
     </row>
@@ -2768,11 +2768,13 @@
       <c r="G41" s="79">
         <v>45210</v>
       </c>
-      <c r="H41" s="80"/>
-      <c r="I41" s="108"/>
+      <c r="H41" s="80">
+        <v>1</v>
+      </c>
+      <c r="I41" s="111"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A42" s="106" t="s">
+      <c r="A42" s="113" t="s">
         <v>122</v>
       </c>
       <c r="B42" s="67" t="s">
@@ -2796,12 +2798,12 @@
       <c r="H42" s="77">
         <v>1</v>
       </c>
-      <c r="I42" s="107"/>
+      <c r="I42" s="110"/>
       <c r="J42" s="9"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A43" s="104"/>
+      <c r="A43" s="108"/>
       <c r="B43" s="68" t="s">
         <v>125</v>
       </c>
@@ -2821,12 +2823,12 @@
         <v>45218</v>
       </c>
       <c r="H43" s="72"/>
-      <c r="I43" s="108"/>
+      <c r="I43" s="111"/>
       <c r="J43" s="9"/>
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A44" s="104"/>
+      <c r="A44" s="108"/>
       <c r="B44" s="69" t="s">
         <v>128</v>
       </c>
@@ -2848,12 +2850,12 @@
       <c r="H44" s="77">
         <v>1</v>
       </c>
-      <c r="I44" s="108"/>
+      <c r="I44" s="111"/>
       <c r="J44" s="9"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A45" s="104"/>
+      <c r="A45" s="108"/>
       <c r="B45" s="61" t="s">
         <v>130</v>
       </c>
@@ -2875,12 +2877,12 @@
       <c r="H45" s="77">
         <v>1</v>
       </c>
-      <c r="I45" s="108"/>
+      <c r="I45" s="111"/>
       <c r="J45" s="9"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A46" s="104"/>
+      <c r="A46" s="108"/>
       <c r="B46" s="61" t="s">
         <v>132</v>
       </c>
@@ -2902,14 +2904,14 @@
       <c r="H46" s="72">
         <v>1</v>
       </c>
-      <c r="I46" s="107" t="s">
+      <c r="I46" s="110" t="s">
         <v>134</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A47" s="104"/>
+      <c r="A47" s="108"/>
       <c r="B47" s="61" t="s">
         <v>87</v>
       </c>
@@ -2931,12 +2933,12 @@
       <c r="H47" s="72">
         <v>1</v>
       </c>
-      <c r="I47" s="108"/>
+      <c r="I47" s="111"/>
       <c r="J47" s="9"/>
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A48" s="104"/>
+      <c r="A48" s="108"/>
       <c r="B48" s="61" t="s">
         <v>91</v>
       </c>
@@ -2958,14 +2960,14 @@
       <c r="H48" s="72">
         <v>1</v>
       </c>
-      <c r="I48" s="107" t="s">
+      <c r="I48" s="110" t="s">
         <v>138</v>
       </c>
       <c r="J48" s="101"/>
       <c r="K48" s="2"/>
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A49" s="105"/>
+      <c r="A49" s="109"/>
       <c r="B49" s="61" t="s">
         <v>139</v>
       </c>
@@ -2987,7 +2989,7 @@
       <c r="H49" s="72">
         <v>1</v>
       </c>
-      <c r="I49" s="108"/>
+      <c r="I49" s="111"/>
       <c r="J49" s="9"/>
       <c r="K49" s="2"/>
     </row>
@@ -3008,7 +3010,7 @@
         <v>45249</v>
       </c>
       <c r="H50" s="82"/>
-      <c r="I50" s="108"/>
+      <c r="I50" s="111"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1">
       <c r="B51" s="11"/>
@@ -4772,11 +4774,6 @@
     <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A10:A25"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I17"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A34:A40"/>
     <mergeCell ref="A42:A49"/>
@@ -4787,6 +4784,11 @@
     <mergeCell ref="I48:I50"/>
     <mergeCell ref="I27:I29"/>
     <mergeCell ref="I31:I33"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A10:A25"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion final del cronograma.
</commit_message>
<xml_diff>
--- a/Línea Base/DPVEI/LB1/DPVEI-CP .xlsx
+++ b/Línea Base/DPVEI/LB1/DPVEI-CP .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unmsmmail-my.sharepoint.com/personal/esteban_quinonez_unmsm_edu_pe/Documents/Escritorio/Tecnofusion/TECNOFUSION/Línea Base/DPVEI/LB1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{EF6AAFA8-7325-4CE1-8989-9C2F03A18181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D47B640-C111-481A-AA72-BBE0E3195CDD}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{EF6AAFA8-7325-4CE1-8989-9C2F03A18181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC055571-EAAE-452F-B5BF-91CB5C819B02}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32040" yWindow="0" windowWidth="17250" windowHeight="9405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -1534,6 +1534,18 @@
     <xf numFmtId="0" fontId="39" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1542,18 +1554,6 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1790,8 +1790,8 @@
   </sheetPr>
   <dimension ref="A1:K1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="C33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1808,23 +1808,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="41.25" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="106"/>
+      <c r="C2" s="112"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -1936,7 +1936,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="113" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="61" t="s">
@@ -1964,7 +1964,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A11" s="108"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="61" t="s">
         <v>21</v>
       </c>
@@ -1986,13 +1986,13 @@
       <c r="H11" s="97">
         <v>1</v>
       </c>
-      <c r="I11" s="110" t="s">
+      <c r="I11" s="107" t="s">
         <v>23</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="108"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="62"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -2000,12 +2000,12 @@
       <c r="F12" s="71"/>
       <c r="G12" s="71"/>
       <c r="H12" s="97"/>
-      <c r="I12" s="111"/>
+      <c r="I12" s="108"/>
       <c r="J12" s="9"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A13" s="108"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="61" t="s">
         <v>24</v>
       </c>
@@ -2027,14 +2027,14 @@
       <c r="H13" s="98">
         <v>1</v>
       </c>
-      <c r="I13" s="110" t="s">
+      <c r="I13" s="107" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="108"/>
+      <c r="A14" s="104"/>
       <c r="B14" s="61" t="s">
         <v>29</v>
       </c>
@@ -2054,11 +2054,11 @@
         <v>45180</v>
       </c>
       <c r="H14" s="99"/>
-      <c r="I14" s="111"/>
+      <c r="I14" s="108"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A15" s="108"/>
+      <c r="A15" s="104"/>
       <c r="B15" s="63" t="s">
         <v>33</v>
       </c>
@@ -2080,11 +2080,11 @@
       <c r="H15" s="97">
         <v>1</v>
       </c>
-      <c r="I15" s="111"/>
+      <c r="I15" s="108"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A16" s="108"/>
+      <c r="A16" s="104"/>
       <c r="B16" s="64" t="s">
         <v>36</v>
       </c>
@@ -2106,12 +2106,12 @@
       <c r="H16" s="97">
         <v>1</v>
       </c>
-      <c r="I16" s="111"/>
+      <c r="I16" s="108"/>
       <c r="J16" s="9"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="108"/>
+      <c r="A17" s="104"/>
       <c r="B17" s="64" t="s">
         <v>38</v>
       </c>
@@ -2133,12 +2133,12 @@
       <c r="H17" s="72">
         <v>1</v>
       </c>
-      <c r="I17" s="111"/>
+      <c r="I17" s="108"/>
       <c r="J17" s="9"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A18" s="108"/>
+      <c r="A18" s="104"/>
       <c r="B18" s="64" t="s">
         <v>41</v>
       </c>
@@ -2165,7 +2165,7 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A19" s="108"/>
+      <c r="A19" s="104"/>
       <c r="B19" s="64" t="s">
         <v>45</v>
       </c>
@@ -2192,7 +2192,7 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A20" s="108"/>
+      <c r="A20" s="104"/>
       <c r="B20" s="64" t="s">
         <v>49</v>
       </c>
@@ -2219,7 +2219,7 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="108"/>
+      <c r="A21" s="104"/>
       <c r="B21" s="64" t="s">
         <v>53</v>
       </c>
@@ -2246,7 +2246,7 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" s="108"/>
+      <c r="A22" s="104"/>
       <c r="B22" s="64" t="s">
         <v>56</v>
       </c>
@@ -2273,7 +2273,7 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" s="108"/>
+      <c r="A23" s="104"/>
       <c r="B23" s="64" t="s">
         <v>59</v>
       </c>
@@ -2300,7 +2300,7 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="108"/>
+      <c r="A24" s="104"/>
       <c r="B24" s="96" t="s">
         <v>62</v>
       </c>
@@ -2327,7 +2327,7 @@
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A25" s="109"/>
+      <c r="A25" s="105"/>
       <c r="B25" s="64" t="s">
         <v>66</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="112" t="s">
+      <c r="A26" s="103" t="s">
         <v>70</v>
       </c>
       <c r="B26" s="64" t="s">
@@ -2383,7 +2383,7 @@
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="108"/>
+      <c r="A27" s="104"/>
       <c r="B27" s="64" t="s">
         <v>75</v>
       </c>
@@ -2405,14 +2405,14 @@
       <c r="H27" s="72">
         <v>1</v>
       </c>
-      <c r="I27" s="110" t="s">
+      <c r="I27" s="107" t="s">
         <v>78</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="108"/>
+      <c r="A28" s="104"/>
       <c r="B28" s="64" t="s">
         <v>79</v>
       </c>
@@ -2434,12 +2434,12 @@
       <c r="H28" s="72">
         <v>1</v>
       </c>
-      <c r="I28" s="111"/>
+      <c r="I28" s="108"/>
       <c r="J28" s="9"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="108"/>
+      <c r="A29" s="104"/>
       <c r="B29" s="65" t="s">
         <v>82</v>
       </c>
@@ -2461,12 +2461,12 @@
       <c r="H29" s="72">
         <v>1</v>
       </c>
-      <c r="I29" s="111"/>
+      <c r="I29" s="108"/>
       <c r="J29" s="9"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="108"/>
+      <c r="A30" s="104"/>
       <c r="B30" s="65" t="s">
         <v>85</v>
       </c>
@@ -2485,7 +2485,7 @@
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="108"/>
+      <c r="A31" s="104"/>
       <c r="B31" s="64" t="s">
         <v>87</v>
       </c>
@@ -2507,14 +2507,14 @@
       <c r="H31" s="72">
         <v>1</v>
       </c>
-      <c r="I31" s="110" t="s">
+      <c r="I31" s="107" t="s">
         <v>90</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A32" s="109"/>
+      <c r="A32" s="105"/>
       <c r="B32" s="64" t="s">
         <v>91</v>
       </c>
@@ -2536,7 +2536,7 @@
       <c r="H32" s="72">
         <v>1</v>
       </c>
-      <c r="I32" s="111"/>
+      <c r="I32" s="108"/>
       <c r="J32" s="9"/>
       <c r="K32" s="2"/>
     </row>
@@ -2557,10 +2557,10 @@
       <c r="H33" s="76">
         <v>1</v>
       </c>
-      <c r="I33" s="111"/>
+      <c r="I33" s="108"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="113" t="s">
+      <c r="A34" s="106" t="s">
         <v>96</v>
       </c>
       <c r="B34" s="67" t="s">
@@ -2581,15 +2581,17 @@
       <c r="G34" s="71">
         <v>45199</v>
       </c>
-      <c r="H34" s="77"/>
-      <c r="I34" s="110" t="s">
+      <c r="H34" s="77">
+        <v>1</v>
+      </c>
+      <c r="I34" s="107" t="s">
         <v>100</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="108"/>
+      <c r="A35" s="104"/>
       <c r="B35" s="67" t="s">
         <v>101</v>
       </c>
@@ -2611,12 +2613,12 @@
       <c r="H35" s="77">
         <v>1</v>
       </c>
-      <c r="I35" s="111"/>
+      <c r="I35" s="108"/>
       <c r="J35" s="9"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="108"/>
+      <c r="A36" s="104"/>
       <c r="B36" s="67" t="s">
         <v>105</v>
       </c>
@@ -2638,12 +2640,12 @@
       <c r="H36" s="77">
         <v>1</v>
       </c>
-      <c r="I36" s="111"/>
+      <c r="I36" s="108"/>
       <c r="J36" s="9"/>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="108"/>
+      <c r="A37" s="104"/>
       <c r="B37" s="64" t="s">
         <v>108</v>
       </c>
@@ -2665,12 +2667,12 @@
       <c r="H37" s="77">
         <v>1</v>
       </c>
-      <c r="I37" s="111"/>
+      <c r="I37" s="108"/>
       <c r="J37" s="9"/>
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A38" s="108"/>
+      <c r="A38" s="104"/>
       <c r="B38" s="64" t="s">
         <v>112</v>
       </c>
@@ -2692,12 +2694,12 @@
       <c r="H38" s="77">
         <v>1</v>
       </c>
-      <c r="I38" s="111"/>
+      <c r="I38" s="108"/>
       <c r="J38" s="9"/>
       <c r="K38" s="100"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="108"/>
+      <c r="A39" s="104"/>
       <c r="B39" s="64" t="s">
         <v>87</v>
       </c>
@@ -2719,14 +2721,14 @@
       <c r="H39" s="77">
         <v>1</v>
       </c>
-      <c r="I39" s="110" t="s">
+      <c r="I39" s="107" t="s">
         <v>117</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="41.25" customHeight="1">
-      <c r="A40" s="109"/>
+      <c r="A40" s="105"/>
       <c r="B40" s="64" t="s">
         <v>91</v>
       </c>
@@ -2748,7 +2750,7 @@
       <c r="H40" s="72">
         <v>1</v>
       </c>
-      <c r="I40" s="111"/>
+      <c r="I40" s="108"/>
       <c r="J40" s="9"/>
       <c r="K40" s="2"/>
     </row>
@@ -2771,10 +2773,10 @@
       <c r="H41" s="80">
         <v>1</v>
       </c>
-      <c r="I41" s="111"/>
+      <c r="I41" s="108"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A42" s="113" t="s">
+      <c r="A42" s="106" t="s">
         <v>122</v>
       </c>
       <c r="B42" s="67" t="s">
@@ -2798,12 +2800,12 @@
       <c r="H42" s="77">
         <v>1</v>
       </c>
-      <c r="I42" s="110"/>
+      <c r="I42" s="107"/>
       <c r="J42" s="9"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A43" s="108"/>
+      <c r="A43" s="104"/>
       <c r="B43" s="68" t="s">
         <v>125</v>
       </c>
@@ -2822,13 +2824,15 @@
       <c r="G43" s="71">
         <v>45218</v>
       </c>
-      <c r="H43" s="72"/>
-      <c r="I43" s="111"/>
+      <c r="H43" s="72">
+        <v>1</v>
+      </c>
+      <c r="I43" s="108"/>
       <c r="J43" s="9"/>
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A44" s="108"/>
+      <c r="A44" s="104"/>
       <c r="B44" s="69" t="s">
         <v>128</v>
       </c>
@@ -2850,12 +2854,12 @@
       <c r="H44" s="77">
         <v>1</v>
       </c>
-      <c r="I44" s="111"/>
+      <c r="I44" s="108"/>
       <c r="J44" s="9"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A45" s="108"/>
+      <c r="A45" s="104"/>
       <c r="B45" s="61" t="s">
         <v>130</v>
       </c>
@@ -2877,12 +2881,12 @@
       <c r="H45" s="77">
         <v>1</v>
       </c>
-      <c r="I45" s="111"/>
+      <c r="I45" s="108"/>
       <c r="J45" s="9"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A46" s="108"/>
+      <c r="A46" s="104"/>
       <c r="B46" s="61" t="s">
         <v>132</v>
       </c>
@@ -2904,14 +2908,14 @@
       <c r="H46" s="72">
         <v>1</v>
       </c>
-      <c r="I46" s="110" t="s">
+      <c r="I46" s="107" t="s">
         <v>134</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A47" s="108"/>
+      <c r="A47" s="104"/>
       <c r="B47" s="61" t="s">
         <v>87</v>
       </c>
@@ -2933,12 +2937,12 @@
       <c r="H47" s="72">
         <v>1</v>
       </c>
-      <c r="I47" s="111"/>
+      <c r="I47" s="108"/>
       <c r="J47" s="9"/>
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A48" s="108"/>
+      <c r="A48" s="104"/>
       <c r="B48" s="61" t="s">
         <v>91</v>
       </c>
@@ -2960,14 +2964,14 @@
       <c r="H48" s="72">
         <v>1</v>
       </c>
-      <c r="I48" s="110" t="s">
+      <c r="I48" s="107" t="s">
         <v>138</v>
       </c>
       <c r="J48" s="101"/>
       <c r="K48" s="2"/>
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A49" s="109"/>
+      <c r="A49" s="105"/>
       <c r="B49" s="61" t="s">
         <v>139</v>
       </c>
@@ -2989,7 +2993,7 @@
       <c r="H49" s="72">
         <v>1</v>
       </c>
-      <c r="I49" s="111"/>
+      <c r="I49" s="108"/>
       <c r="J49" s="9"/>
       <c r="K49" s="2"/>
     </row>
@@ -3010,7 +3014,7 @@
         <v>45249</v>
       </c>
       <c r="H50" s="82"/>
-      <c r="I50" s="111"/>
+      <c r="I50" s="108"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1">
       <c r="B51" s="11"/>
@@ -4774,6 +4778,11 @@
     <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A10:A25"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I17"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="A34:A40"/>
     <mergeCell ref="A42:A49"/>
@@ -4784,11 +4793,6 @@
     <mergeCell ref="I48:I50"/>
     <mergeCell ref="I27:I29"/>
     <mergeCell ref="I31:I33"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A10:A25"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>